<commit_message>
Updates for TDS version
</commit_message>
<xml_diff>
--- a/Contoso - Sales - Current Release/Dataverse Data/1 🎯Campaigns for Import.xlsx
+++ b/Contoso - Sales - Current Release/Dataverse Data/1 🎯Campaigns for Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/misewell_microsoft_com/Documents/Documents/GitHub/ContosoBI/Contoso - Sales - Current Release/Dataverse Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_A003BFCDDD72B981B778627203929DF7A49BAB1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB30B2A0-78A7-4463-9AF8-95D0D6A57A31}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_A003BFCDDD72B981B778627203929DF7A49BAB1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{220DCEF4-2157-44F2-A7A5-DA4F5467968F}"/>
   <bookViews>
-    <workbookView xWindow="61995" yWindow="1470" windowWidth="23085" windowHeight="15630" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My Campaigns" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>(Do Not Modify) Campaign</t>
   </si>
@@ -69,44 +69,65 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Ad campaign template</t>
-  </si>
-  <si>
-    <t>Co-branding with large retailer</t>
-  </si>
-  <si>
-    <t>Direct marketing template</t>
-  </si>
-  <si>
-    <t>Event campaign template</t>
-  </si>
-  <si>
-    <t>New customer loyalty program</t>
-  </si>
-  <si>
-    <t>Product launch campaign</t>
-  </si>
-  <si>
-    <t>Charity event</t>
-  </si>
-  <si>
-    <t>New ad campaign</t>
+    <t>Café A-100 Automatic plus Coffee Beans</t>
+  </si>
+  <si>
+    <t>Café A-100 Automatic plus Coffee Cloud Subscription</t>
+  </si>
+  <si>
+    <t>Café S-200 Semiautomatic plus Service Agreement</t>
+  </si>
+  <si>
+    <t>Smart Brew 300 plus Coffee Beans</t>
+  </si>
+  <si>
+    <t>Café PG-1 Professional plus Coffee Cloud Subscription</t>
+  </si>
+  <si>
+    <t>Customer Reference Lead</t>
+  </si>
+  <si>
+    <t>Market Trends Newsletter</t>
+  </si>
+  <si>
+    <t>Monthly Newsletter</t>
+  </si>
+  <si>
+    <t>New Product Releases</t>
+  </si>
+  <si>
+    <t>Search Results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Game Sponsorship </t>
+  </si>
+  <si>
+    <t>In-App Video Placement</t>
+  </si>
+  <si>
+    <t>Customer Care Campaign</t>
+  </si>
+  <si>
+    <t>Customer Follow-up</t>
+  </si>
+  <si>
+    <t>Commercial Tradeshow</t>
+  </si>
+  <si>
+    <t>Consumer Tradeshow</t>
+  </si>
+  <si>
+    <t>QuarterlySales Contest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -118,12 +139,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9E1F2"/>
-        <bgColor rgb="FFD9E1F2"/>
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -131,16 +152,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -206,8 +252,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E9" totalsRowShown="0">
-  <autoFilter ref="A1:E9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:E18" totalsRowShown="0">
+  <autoFilter ref="A1:E18" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E9">
+    <sortCondition ref="E1:E9"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Campaign"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
@@ -220,9 +269,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -260,7 +309,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -366,7 +415,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -508,7 +557,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -517,13 +566,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E9" sqref="D2:E9"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
@@ -532,7 +581,7 @@
     <col min="5" max="5" width="35" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,68 +598,140 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5">
       <c r="D2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="D5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="4" t="s">
+    <row r="12" spans="1:5">
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
+    <row r="17" spans="4:5">
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D9" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
+    <row r="18" spans="4:5">
+      <c r="D18" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -648,14 +769,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Updated per changes from design team.
</commit_message>
<xml_diff>
--- a/Contoso - Sales - Current Release/Dataverse Data/1 🎯Campaigns for Import.xlsx
+++ b/Contoso - Sales - Current Release/Dataverse Data/1 🎯Campaigns for Import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/misewell_microsoft_com/Documents/Documents/GitHub/ContosoBI/Contoso - Sales - Current Release/Dataverse Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_A003BFCDDD72B981B778627203929DF7A49BAB1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{220DCEF4-2157-44F2-A7A5-DA4F5467968F}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_A003BFCDDD72B981B778627203929DF7A49BAB1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B715BA7-5F53-4438-A2B8-85B35F4A66A4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="30220" windowHeight="19500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="50010" yWindow="2520" windowWidth="43200" windowHeight="23325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My Campaigns" sheetId="1" r:id="rId1"/>
@@ -124,27 +124,21 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor theme="5" tint="0.79998168889431442"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -152,93 +146,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </right>
-      <top style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="thin">
-        <color theme="5" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9E1F2"/>
-          <bgColor rgb="FFD9E1F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFD9E1F2"/>
-          <bgColor rgb="FFD9E1F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -261,8 +181,8 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Campaign"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(Do Not Modify) Modified On"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Name" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Campaign Type" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Name" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Campaign Type" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -569,10 +489,10 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
@@ -581,7 +501,7 @@
     <col min="5" max="5" width="35" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -598,47 +518,47 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="D3" s="5" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="D4" s="3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="D5" s="5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
-      <c r="D6" s="3" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>16</v>
       </c>
@@ -646,7 +566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
         <v>17</v>
       </c>
@@ -654,7 +574,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
         <v>18</v>
       </c>
@@ -662,7 +582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
         <v>19</v>
       </c>
@@ -670,7 +590,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
         <v>20</v>
       </c>
@@ -678,7 +598,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
         <v>21</v>
       </c>
@@ -686,7 +606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
         <v>22</v>
       </c>
@@ -694,7 +614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
         <v>23</v>
       </c>
@@ -702,7 +622,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
         <v>24</v>
       </c>
@@ -710,7 +630,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
         <v>25</v>
       </c>
@@ -718,7 +638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>26</v>
       </c>
@@ -726,7 +646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>27</v>
       </c>
@@ -769,14 +689,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update TDS-Based Reports and Installation Instructions
</commit_message>
<xml_diff>
--- a/Contoso - Sales - Current Release/Dataverse Data/1 🎯Campaigns for Import.xlsx
+++ b/Contoso - Sales - Current Release/Dataverse Data/1 🎯Campaigns for Import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://microsoft-my.sharepoint.com/personal/misewell_microsoft_com/Documents/Documents/GitHub/ContosoBI/Contoso - Sales - Current Release/Dataverse Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\misewell\Documents\GitHub\ContosoBI\Contoso - Sales - Current Release\Dataverse Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_A003BFCDDD72B981B778627203929DF7A49BAB1D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7B715BA7-5F53-4438-A2B8-85B35F4A66A4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03BB998E-6D45-4E56-B621-40E0929AD77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50010" yWindow="2520" windowWidth="43200" windowHeight="23325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1650" yWindow="1740" windowWidth="33180" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="My Campaigns" sheetId="1" r:id="rId1"/>
@@ -69,21 +69,6 @@
     <t>Other</t>
   </si>
   <si>
-    <t>Café A-100 Automatic plus Coffee Beans</t>
-  </si>
-  <si>
-    <t>Café A-100 Automatic plus Coffee Cloud Subscription</t>
-  </si>
-  <si>
-    <t>Café S-200 Semiautomatic plus Service Agreement</t>
-  </si>
-  <si>
-    <t>Smart Brew 300 plus Coffee Beans</t>
-  </si>
-  <si>
-    <t>Café PG-1 Professional plus Coffee Cloud Subscription</t>
-  </si>
-  <si>
     <t>Customer Reference Lead</t>
   </si>
   <si>
@@ -118,6 +103,21 @@
   </si>
   <si>
     <t>QuarterlySales Contest</t>
+  </si>
+  <si>
+    <t>Le Tour Bundle</t>
+  </si>
+  <si>
+    <t>Family Bike Collection</t>
+  </si>
+  <si>
+    <t>Commuter Special</t>
+  </si>
+  <si>
+    <t>Tube Advert Special</t>
+  </si>
+  <si>
+    <t>ProAm Collection</t>
   </si>
 </sst>
 </file>
@@ -181,15 +181,15 @@
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Campaign"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(Do Not Modify) Modified On"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Name" dataCellStyle="Normal"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Campaign Type" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Name"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Campaign Type"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -477,7 +477,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -489,7 +489,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -497,7 +497,7 @@
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="0" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="62" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.1796875" style="1" customWidth="1"/>
     <col min="5" max="5" width="35" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -531,7 +531,7 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -539,7 +539,7 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -547,7 +547,7 @@
         <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -555,20 +555,20 @@
         <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -576,23 +576,23 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -600,15 +600,15 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
@@ -616,42 +616,42 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>